<commit_message>
Laporan anev preview html done
</commit_message>
<xml_diff>
--- a/public/template/excel/absensi_update.xlsx
+++ b/public/template/excel/absensi_update.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>MARKAS BESAR</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>DATA ABSENSI POLDA</t>
-  </si>
-  <si>
-    <t>TANGGAL 18 NOVEMBER 2021</t>
   </si>
   <si>
     <t>NOMOR</t>
@@ -676,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="178" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -731,9 +728,7 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -743,13 +738,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -757,10 +752,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -768,10 +763,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -779,10 +774,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -790,10 +785,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -801,10 +796,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,10 +807,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -823,10 +818,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -834,10 +829,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,10 +840,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -856,10 +851,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -867,10 +862,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -878,10 +873,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,10 +884,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,10 +895,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -911,10 +906,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -922,10 +917,10 @@
         <v>16</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -933,10 +928,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,10 +939,10 @@
         <v>18</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -955,10 +950,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,10 +961,10 @@
         <v>20</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -977,10 +972,10 @@
         <v>21</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,10 +983,10 @@
         <v>22</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,10 +994,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1010,10 +1005,10 @@
         <v>24</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,10 +1016,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,10 +1027,10 @@
         <v>26</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,10 +1038,10 @@
         <v>27</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1054,10 +1049,10 @@
         <v>28</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1065,10 +1060,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,10 +1071,10 @@
         <v>30</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,10 +1082,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,10 +1093,10 @@
         <v>32</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,10 +1104,10 @@
         <v>33</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1120,10 +1115,10 @@
         <v>34</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">

</xml_diff>